<commit_message>
Zweite Version mit ActionListenern und erster Logik.
</commit_message>
<xml_diff>
--- a/resources/Menü.xlsx
+++ b/resources/Menü.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\2 Java\LF-ZQ16a OOP mit Java\Übungen\SwingPizza\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6E3AAC-AF49-4AB2-850F-64E1A8EC15AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20F955A-19E9-4DE9-B83B-0F250B35CE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31755" yWindow="1680" windowWidth="21600" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-15" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menü" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Nr</t>
   </si>
@@ -43,18 +43,12 @@
     <t>Margherita</t>
   </si>
   <si>
-    <t>Tomaten und Käse</t>
-  </si>
-  <si>
     <t>Salami</t>
   </si>
   <si>
     <t>Prosciutto</t>
   </si>
   <si>
-    <t>Schinken</t>
-  </si>
-  <si>
     <t>Größe</t>
   </si>
   <si>
@@ -94,28 +88,46 @@
     <t>https://cdn.pixabay.com/photo/2024/01/21/21/38/ai-generated-8524058_640.jpg</t>
   </si>
   <si>
-    <t>https://pixabay.com/get/g109ca7a312cf47391a875c7cbbdc9e4bfec09765e153ed7e3fbc5010b0c16f62562d481cf02841e918674dbcb277cf755248b95ef9358a2c43419f59a3315bb5f5bcf67582a6305ec14849d07fc21a57_640.jpg</t>
-  </si>
-  <si>
-    <t>https://pixabay.com/get/g0094f9719f09f1a95a4dfe02ca54521758c4481ad492e6a6b6b181e758814052cf178b4cacc521f02cc32162ac1973eb0c1ab0addc155ae6c18f3c1c5b39f314b5d163c853d1e0a0f0a58c8a65af0d6d_640.jpg</t>
-  </si>
-  <si>
     <t>Funghi</t>
   </si>
   <si>
-    <t>Pilze</t>
-  </si>
-  <si>
-    <t>https://pixabay.com/get/g41c3ec10f8eef0878e834a3bc94d0111bd1854f1328507b3039fac8910c1f0847edc9a7fe63d9d85b1b5a0a7714994163dcf7ec38a8ac534284913a91b8873d1bbadb7ae5595212b6aded112a810b996_640.jpg</t>
-  </si>
-  <si>
     <t>Tonno</t>
   </si>
   <si>
-    <t>Thunfisch und Zwiebeln</t>
-  </si>
-  <si>
-    <t>https://www.koch-mit.de/app/uploads/2023/01/thunfisch_pizza_titel.jpg</t>
+    <t>https://kungfu-pizza.ro/wp-content/uploads/2020/12/pizza-salami.jpg</t>
+  </si>
+  <si>
+    <t>https://as2.ftcdn.net/v2/jpg/04/80/82/95/1000_F_480829568_QySaJtZXCxPULUZ3CFiyDIrnuxQ85Of9.jpg</t>
+  </si>
+  <si>
+    <t>https://www.eatbetter.de/sites/eatbetter.de/files/styles/facebook/public/2023-04/pizza_funghi_8823.jpg?h=4521fff0&amp;itok=XcDJ5gFv</t>
+  </si>
+  <si>
+    <t>https://www.globus.de/media/globus/rezepte/globus/pizza_tonno_169.jpg</t>
+  </si>
+  <si>
+    <t>mit frischen Tomaten, Basillikum und Käse</t>
+  </si>
+  <si>
+    <t>mit Salami und Käse</t>
+  </si>
+  <si>
+    <t>mit Schinken und Käse</t>
+  </si>
+  <si>
+    <t>mit frischen Pilzen</t>
+  </si>
+  <si>
+    <t>mit Thunfisch und Zwiebeln</t>
+  </si>
+  <si>
+    <t>Capricciosa</t>
+  </si>
+  <si>
+    <t>mit Artischocken, Pilzen, Schinken und schwarzen Oliven</t>
+  </si>
+  <si>
+    <t>https://www.italianstylecooking.net/wp-content/uploads/2022/01/Pizza-capricciosa.jpg</t>
   </si>
 </sst>
 </file>
@@ -168,17 +180,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -460,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,92 +511,109 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="6">
+        <v>5.99</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2">
-        <v>5.99</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="C3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4">
+        <v>6.99</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="4">
+        <v>6.99</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4">
+        <v>6.99</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4">
+        <v>6.99</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>6.99</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>6.99</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5">
-        <v>6.99</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6">
-        <v>6.99</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>29</v>
+      <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4">
+        <v>7.99</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -580,8 +621,7 @@
     <hyperlink ref="E2" r:id="rId1" xr:uid="{1C93AA11-BD1C-4F2B-BBAD-17A221625FDC}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{FED48BBF-4F73-4E66-8618-E2F58D0477F4}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{C7B7F7C1-DA8E-4F05-93F7-0B38D472B6B4}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{E612F426-5461-4537-9740-CF245885833A}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{C59D6CA3-EFD1-4F29-A675-DE59EA63009C}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{33F09566-9D71-46C3-AB5F-A8B2D3526018}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -599,21 +639,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2">
         <v>-1</v>
@@ -621,10 +661,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
@@ -632,10 +672,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -643,10 +683,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2">
         <v>3</v>

</xml_diff>